<commit_message>
Removed old Usings Added New Strings Modified Person Table Straightened Out Upload page Added FLight Schema Until we get Beeter PEX Data Modified PEX Ingest
</commit_message>
<xml_diff>
--- a/Mock Data/PEX.xlsx
+++ b/Mock Data/PEX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24301"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\OneDrive\Documents\kunaikode\Mock Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED2CA18-8A67-45A5-B8BA-27D2BA5B8DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5064BCCF-3F52-4D5C-9CF7-92E7996F7D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="2565" windowWidth="19995" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1890" yWindow="4800" windowWidth="34590" windowHeight="15525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>ChurchillO</t>
   </si>
   <si>
-    <t>McLeanA</t>
-  </si>
-  <si>
     <t>MitchellJ</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>IRF 6 / 1</t>
+  </si>
+  <si>
+    <t>McleanA</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -461,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,7 +477,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -485,7 +485,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +493,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,71 +501,71 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>